<commit_message>
Floyd Wallace fix subscription_switch to add custom line item properties product_collection when customer switches products so vishy code can fullfil
</commit_message>
<xml_diff>
--- a/alternate_products.xlsx
+++ b/alternate_products.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>product_title</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Modern Muse - 5 Item</t>
+  </si>
+  <si>
+    <t>product_collection</t>
   </si>
 </sst>
 </file>
@@ -415,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -429,7 +432,7 @@
     <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -442,8 +445,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -456,8 +462,11 @@
       <c r="D2" s="1">
         <v>764204108572</v>
       </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -470,8 +479,11 @@
       <c r="D3" s="1">
         <v>764204108565</v>
       </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -484,8 +496,11 @@
       <c r="D4" s="1">
         <v>764204046874</v>
       </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -498,8 +513,11 @@
       <c r="D5" s="1">
         <v>764204046867</v>
       </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>

</xml_diff>